<commit_message>
added final IPC CAR and Guinea results
</commit_message>
<xml_diff>
--- a/data/fiche_comm/adm0_fiche_comm.xlsx
+++ b/data/fiche_comm/adm0_fiche_comm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RBD_CHIPC_dataprocessing\data\fiche_comm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC3D053-C67C-408A-95C4-9AD19380AC0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B5F967-3EA5-4C33-B990-14D88F82D11B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="adm0" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4280" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4280" uniqueCount="126">
   <si>
     <t>adm0_pcod3</t>
   </si>
@@ -410,10 +410,13 @@
     <t>CH-SN mars 21</t>
   </si>
   <si>
-    <t>draft figures - to be updated with finalized figures</t>
+    <t xml:space="preserve">Projected </t>
   </si>
   <si>
-    <t xml:space="preserve">Projected </t>
+    <t>CAR-Projection Update April 2021-Pop Table</t>
+  </si>
+  <si>
+    <t>Tableur 4-CH-GN-RQQ 05052021</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -770,6 +773,11 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1010,8 +1018,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AN996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P539" sqref="P539"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S543" sqref="S543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2151,7 +2159,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -2199,7 +2207,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -3420,7 +3428,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:40" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>37</v>
       </c>
@@ -4940,7 +4948,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>37</v>
       </c>
@@ -4988,7 +4996,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>37</v>
       </c>
@@ -6545,7 +6553,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>37</v>
       </c>
@@ -6599,7 +6607,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>37</v>
       </c>
@@ -8327,7 +8335,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>37</v>
       </c>
@@ -8375,7 +8383,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>37</v>
       </c>
@@ -10069,7 +10077,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>37</v>
       </c>
@@ -10123,7 +10131,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>37</v>
       </c>
@@ -12052,7 +12060,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>37</v>
       </c>
@@ -12111,7 +12119,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>37</v>
       </c>
@@ -14192,7 +14200,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
         <v>37</v>
       </c>
@@ -14254,7 +14262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
         <v>37</v>
       </c>
@@ -16300,7 +16308,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="4" t="s">
         <v>37</v>
       </c>
@@ -16362,7 +16370,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="281" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="4" t="s">
         <v>37</v>
       </c>
@@ -18514,7 +18522,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="316" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="4" t="s">
         <v>37</v>
       </c>
@@ -18576,7 +18584,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="317" spans="1:21" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="27" t="s">
         <v>37</v>
       </c>
@@ -20756,7 +20764,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="352" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="27" t="s">
         <v>37</v>
       </c>
@@ -20818,7 +20826,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="353" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="27" t="s">
         <v>37</v>
       </c>
@@ -23049,7 +23057,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="389" spans="1:40" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="4" t="s">
         <v>37</v>
       </c>
@@ -25297,7 +25305,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="424" spans="1:40" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A424" s="4" t="s">
         <v>37</v>
       </c>
@@ -25359,7 +25367,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="425" spans="1:40" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A425" s="4" t="s">
         <v>37</v>
       </c>
@@ -27958,7 +27966,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="466" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A466" s="4" t="s">
         <v>37</v>
       </c>
@@ -28020,7 +28028,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="467" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A467" s="4" t="s">
         <v>37</v>
       </c>
@@ -29755,7 +29763,7 @@
         <v>2019</v>
       </c>
       <c r="G495" s="78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H495" s="78">
         <v>2</v>
@@ -30111,65 +30119,65 @@
         <v>63</v>
       </c>
     </row>
-    <row r="501" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A501" s="4" t="s">
+    <row r="501" spans="1:21" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A501" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B501" s="44">
+      <c r="B501" s="81">
         <v>106</v>
       </c>
-      <c r="C501" s="45" t="s">
+      <c r="C501" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="D501" s="4">
-        <v>2</v>
-      </c>
-      <c r="E501" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F501" s="4">
+      <c r="D501" s="56">
+        <v>2</v>
+      </c>
+      <c r="E501" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="F501" s="56">
         <v>2021</v>
       </c>
-      <c r="G501" s="4" t="s">
+      <c r="G501" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="H501" s="4">
-        <v>2</v>
-      </c>
-      <c r="I501" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="J501" s="4">
+      <c r="H501" s="56">
+        <v>2</v>
+      </c>
+      <c r="I501" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="J501" s="56">
         <v>2021</v>
       </c>
-      <c r="K501" s="16">
-        <v>0</v>
-      </c>
-      <c r="L501" s="16">
-        <v>0</v>
-      </c>
-      <c r="M501" s="16">
-        <v>0</v>
-      </c>
-      <c r="N501" s="16">
-        <v>0</v>
-      </c>
-      <c r="O501" s="16">
-        <v>0</v>
-      </c>
-      <c r="P501" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q501" s="16">
-        <v>0</v>
-      </c>
-      <c r="R501" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="S501" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="U501" s="4" t="s">
+      <c r="K501" s="68">
+        <v>11115573</v>
+      </c>
+      <c r="L501" s="25">
+        <v>8235003.6000000015</v>
+      </c>
+      <c r="M501" s="25">
+        <v>2426627.8200000003</v>
+      </c>
+      <c r="N501" s="25">
+        <v>453941.58000000013</v>
+      </c>
+      <c r="O501" s="25">
+        <v>0</v>
+      </c>
+      <c r="P501" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q501" s="25">
+        <v>453941.58000000013</v>
+      </c>
+      <c r="R501" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="S501" s="83" t="s">
+        <v>125</v>
+      </c>
+      <c r="U501" s="56" t="s">
         <v>63</v>
       </c>
     </row>
@@ -30359,7 +30367,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="505" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A505" s="4" t="s">
         <v>47</v>
       </c>
@@ -31112,65 +31120,65 @@
         <v>63</v>
       </c>
     </row>
-    <row r="517" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A517" s="4" t="s">
+    <row r="517" spans="1:21" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A517" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B517" s="44">
+      <c r="B517" s="81">
         <v>106</v>
       </c>
-      <c r="C517" s="45" t="s">
+      <c r="C517" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="D517" s="4">
-        <v>2</v>
-      </c>
-      <c r="E517" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F517" s="4">
+      <c r="D517" s="56">
+        <v>2</v>
+      </c>
+      <c r="E517" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="F517" s="56">
         <v>2021</v>
       </c>
-      <c r="G517" s="4" t="s">
+      <c r="G517" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="H517" s="4">
+      <c r="H517" s="56">
         <v>3</v>
       </c>
-      <c r="I517" s="4" t="s">
+      <c r="I517" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="J517" s="4">
+      <c r="J517" s="56">
         <v>2021</v>
       </c>
-      <c r="K517" s="16">
+      <c r="K517" s="25">
         <v>11115573</v>
       </c>
-      <c r="L517" s="16">
-        <v>8262248.0599999996</v>
-      </c>
-      <c r="M517" s="16">
-        <v>2169692.1600000001</v>
-      </c>
-      <c r="N517" s="16">
-        <v>683632.78000000014</v>
-      </c>
-      <c r="O517" s="16">
-        <v>0</v>
-      </c>
-      <c r="P517" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q517" s="16">
-        <v>683632.78000000014</v>
-      </c>
-      <c r="R517" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="S517" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="U517" s="4" t="s">
+      <c r="L517" s="25">
+        <v>8124709.3299999991</v>
+      </c>
+      <c r="M517" s="25">
+        <v>2572410.3000000007</v>
+      </c>
+      <c r="N517" s="25">
+        <v>418453.36999999994</v>
+      </c>
+      <c r="O517" s="25">
+        <v>0</v>
+      </c>
+      <c r="P517" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q517" s="25">
+        <v>418453.36999999994</v>
+      </c>
+      <c r="R517" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="S517" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="U517" s="56" t="s">
         <v>63</v>
       </c>
     </row>
@@ -31360,7 +31368,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="521" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A521" s="4" t="s">
         <v>47</v>
       </c>
@@ -32013,7 +32021,7 @@
         <v>2020</v>
       </c>
       <c r="G531" s="78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H531" s="78">
         <v>2</v>
@@ -32048,8 +32056,8 @@
       <c r="R531" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="S531" s="78" t="s">
-        <v>123</v>
+      <c r="S531" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="U531" s="78" t="s">
         <v>63</v>
@@ -32091,27 +32099,32 @@
       <c r="J533" s="69">
         <v>2021</v>
       </c>
-      <c r="K533" s="73"/>
-      <c r="L533" s="74"/>
-      <c r="M533" s="74"/>
+      <c r="K533" s="73">
+        <v>4879385</v>
+      </c>
+      <c r="L533" s="74">
+        <v>998450</v>
+      </c>
+      <c r="M533" s="74">
+        <v>1591200</v>
+      </c>
       <c r="N533" s="75">
-        <v>1657213</v>
+        <v>1657212</v>
       </c>
       <c r="O533" s="76">
-        <v>632525</v>
-      </c>
-      <c r="P533" s="25">
+        <v>632524</v>
+      </c>
+      <c r="P533" s="16">
         <v>0</v>
       </c>
       <c r="Q533" s="25">
-        <f>SUM(N533:O533)</f>
-        <v>2289738</v>
+        <v>2289736</v>
       </c>
       <c r="R533" s="56" t="s">
         <v>26</v>
       </c>
       <c r="S533" s="56" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="U533" s="56" t="s">
         <v>63</v>
@@ -32586,15 +32599,10 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:AN534" xr:uid="{39ABAFED-046F-4AC9-B50A-A3F0F0F18739}">
+  <autoFilter ref="A1:AN534" xr:uid="{4A94B884-F025-45F8-8A74-6143E218625F}">
     <filterColumn colId="0">
       <filters>
-        <filter val="MRT"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="2021"/>
+        <filter val="GIN"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>